<commit_message>
select data source work
</commit_message>
<xml_diff>
--- a/Resources/certificationDataTemplate.xlsx
+++ b/Resources/certificationDataTemplate.xlsx
@@ -633,26 +633,224 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
+  <dxfs count="28">
+    <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -684,224 +882,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -910,46 +890,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="75" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -1155,6 +1095,66 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="75" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -1164,90 +1164,40 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H6" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowBorderDxfId="31" tableBorderDxfId="32" totalsRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H6" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="A1:H6"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Discipline" dataDxfId="26"/>
-    <tableColumn id="2" name="Vision" dataDxfId="25"/>
-    <tableColumn id="3" name="Level One Chair Umpire" dataDxfId="24"/>
-    <tableColumn id="4" name="Level One Line Umpire" dataDxfId="23"/>
-    <tableColumn id="5" name="Level One Referee Course" dataDxfId="22"/>
-    <tableColumn id="6" name="Level One Roving Umpire Course" dataDxfId="21"/>
-    <tableColumn id="7" name="Level Two Referee" dataDxfId="20"/>
-    <tableColumn id="8" name="Level Two Roving Umpire" dataDxfId="19"/>
+    <tableColumn id="1" name="Discipline" dataDxfId="21"/>
+    <tableColumn id="2" name="Vision" dataDxfId="20"/>
+    <tableColumn id="3" name="Level One Chair Umpire" dataDxfId="19"/>
+    <tableColumn id="4" name="Level One Line Umpire" dataDxfId="18"/>
+    <tableColumn id="5" name="Level One Referee Course" dataDxfId="17"/>
+    <tableColumn id="6" name="Level One Roving Umpire Course" dataDxfId="16"/>
+    <tableColumn id="7" name="Level Two Referee" dataDxfId="15"/>
+    <tableColumn id="8" name="Level Two Roving Umpire" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H33" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H33" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A1:H33"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="First Name" dataDxfId="11"/>
-    <tableColumn id="2" name="Last Name" dataDxfId="10"/>
-    <tableColumn id="3" name="Email" dataDxfId="9" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" name="Roving Umpire (Sectional)" dataDxfId="8"/>
-    <tableColumn id="5" name="Roving Umpire (USTA)" dataDxfId="7"/>
-    <tableColumn id="6" name="Chair Umpire (Sectional, USTA, National, Professional)" dataDxfId="6"/>
-    <tableColumn id="7" name="Referee (Sectional, USTA, National, Professional)" dataDxfId="5"/>
-    <tableColumn id="8" name="Line Umpire (USTA, National, Professional)" dataDxfId="4"/>
+    <tableColumn id="1" name="First Name" dataDxfId="7"/>
+    <tableColumn id="2" name="Last Name" dataDxfId="6"/>
+    <tableColumn id="3" name="Email" dataDxfId="5" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="Roving Umpire (Sectional)" dataDxfId="4"/>
+    <tableColumn id="5" name="Roving Umpire (USTA)" dataDxfId="3"/>
+    <tableColumn id="6" name="Chair Umpire (Sectional, USTA, National, Professional)" dataDxfId="2"/>
+    <tableColumn id="7" name="Referee (Sectional, USTA, National, Professional)" dataDxfId="1"/>
+    <tableColumn id="8" name="Line Umpire (USTA, National, Professional)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1578,7 +1528,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1588,7 +1538,7 @@
     <col min="9" max="16384" width="10.83203125" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="15" customFormat="1" ht="167">
+    <row r="1" spans="1:8" s="15" customFormat="1" ht="181" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>75</v>
       </c>
@@ -1749,7 +1699,7 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="A2:AW498">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1779,8 +1729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1792,7 +1742,7 @@
     <col min="10" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="270">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="264">
       <c r="A1" s="30" t="s">
         <v>78</v>
       </c>
@@ -2652,7 +2602,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:H500 I2:AP499">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
process officials module handles disciplines
</commit_message>
<xml_diff>
--- a/Resources/certificationDataTemplate.xlsx
+++ b/Resources/certificationDataTemplate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
   <si>
     <t>Level One Referee Course</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>First Name</t>
+  </si>
+  <si>
+    <t>name of another</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -481,8 +484,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -586,8 +592,14 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="37" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="75"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -612,6 +624,9 @@
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -635,6 +650,26 @@
   </cellStyles>
   <dxfs count="28">
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -646,16 +681,26 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -669,34 +714,7 @@
         <left style="thin">
           <color auto="1"/>
         </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
+        <right/>
         <top style="thin">
           <color auto="1"/>
         </top>
@@ -880,16 +898,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -1154,50 +1162,39 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H6" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H6" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="A1:H6"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Discipline" dataDxfId="21"/>
-    <tableColumn id="2" name="Vision" dataDxfId="20"/>
-    <tableColumn id="3" name="Level One Chair Umpire" dataDxfId="19"/>
-    <tableColumn id="4" name="Level One Line Umpire" dataDxfId="18"/>
-    <tableColumn id="5" name="Level One Referee Course" dataDxfId="17"/>
-    <tableColumn id="6" name="Level One Roving Umpire Course" dataDxfId="16"/>
-    <tableColumn id="7" name="Level Two Referee" dataDxfId="15"/>
-    <tableColumn id="8" name="Level Two Roving Umpire" dataDxfId="14"/>
+    <tableColumn id="1" name="Discipline" dataDxfId="22"/>
+    <tableColumn id="2" name="Vision" dataDxfId="21"/>
+    <tableColumn id="3" name="Level One Chair Umpire" dataDxfId="20"/>
+    <tableColumn id="4" name="Level One Line Umpire" dataDxfId="19"/>
+    <tableColumn id="5" name="Level One Referee Course" dataDxfId="18"/>
+    <tableColumn id="6" name="Level One Roving Umpire Course" dataDxfId="17"/>
+    <tableColumn id="7" name="Level Two Referee" dataDxfId="16"/>
+    <tableColumn id="8" name="Level Two Roving Umpire" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H33" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="A1:H33"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="First Name" dataDxfId="7"/>
-    <tableColumn id="2" name="Last Name" dataDxfId="6"/>
-    <tableColumn id="3" name="Email" dataDxfId="5" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" name="Roving Umpire (Sectional)" dataDxfId="4"/>
-    <tableColumn id="5" name="Roving Umpire (USTA)" dataDxfId="3"/>
-    <tableColumn id="6" name="Chair Umpire (Sectional, USTA, National, Professional)" dataDxfId="2"/>
-    <tableColumn id="7" name="Referee (Sectional, USTA, National, Professional)" dataDxfId="1"/>
-    <tableColumn id="8" name="Line Umpire (USTA, National, Professional)" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G33" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="A1:G33"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="First Name" dataDxfId="9"/>
+    <tableColumn id="2" name="Last Name" dataDxfId="8"/>
+    <tableColumn id="3" name="Email" dataDxfId="7" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="Roving Umpire (Sectional)" dataDxfId="6"/>
+    <tableColumn id="7" name="Referee (Sectional, USTA, National, Professional)" dataDxfId="5"/>
+    <tableColumn id="8" name="name of another" dataDxfId="4"/>
+    <tableColumn id="9" name="Roving Umpire (USTA)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1699,7 +1696,7 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="A2:AW498">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1727,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1738,11 +1735,11 @@
     <col min="1" max="1" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="4.83203125" style="9" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="9"/>
+    <col min="4" max="7" width="4.83203125" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="264">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="244">
       <c r="A1" s="30" t="s">
         <v>78</v>
       </c>
@@ -1756,19 +1753,16 @@
         <v>7</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="28" t="s">
         <v>12</v>
       </c>
@@ -1784,17 +1778,14 @@
       <c r="E2" s="8">
         <v>0</v>
       </c>
-      <c r="F2" s="8">
-        <v>0</v>
-      </c>
-      <c r="G2" s="8">
-        <v>0</v>
-      </c>
-      <c r="H2" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="F2" s="17">
+        <v>0</v>
+      </c>
+      <c r="G2" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="28" t="s">
         <v>13</v>
       </c>
@@ -1810,17 +1801,14 @@
       <c r="E3" s="8">
         <v>0</v>
       </c>
-      <c r="F3" s="8">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0</v>
-      </c>
-      <c r="H3" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="F3" s="17">
+        <v>1</v>
+      </c>
+      <c r="G3" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="28" t="s">
         <v>14</v>
       </c>
@@ -1834,19 +1822,16 @@
         <v>0</v>
       </c>
       <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0</v>
-      </c>
-      <c r="G4" s="8">
-        <v>1</v>
-      </c>
-      <c r="H4" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="17">
+        <v>0</v>
+      </c>
+      <c r="G4" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="28" t="s">
         <v>15</v>
       </c>
@@ -1860,19 +1845,16 @@
         <v>0</v>
       </c>
       <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>1</v>
-      </c>
-      <c r="H5" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="17">
+        <v>1</v>
+      </c>
+      <c r="G5" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="28" t="s">
         <v>16</v>
       </c>
@@ -1888,17 +1870,14 @@
       <c r="E6" s="8">
         <v>0</v>
       </c>
-      <c r="F6" s="8">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="F6" s="17">
+        <v>0</v>
+      </c>
+      <c r="G6" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="28" t="s">
         <v>17</v>
       </c>
@@ -1914,17 +1893,14 @@
       <c r="E7" s="8">
         <v>0</v>
       </c>
-      <c r="F7" s="8">
-        <v>1</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-      <c r="H7" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="F7" s="17">
+        <v>1</v>
+      </c>
+      <c r="G7" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="28" t="s">
         <v>18</v>
       </c>
@@ -1938,19 +1914,16 @@
         <v>0</v>
       </c>
       <c r="E8" s="8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0</v>
+      </c>
+      <c r="G8" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="28" t="s">
         <v>19</v>
       </c>
@@ -1964,19 +1937,16 @@
         <v>0</v>
       </c>
       <c r="E9" s="8">
-        <v>0</v>
-      </c>
-      <c r="F9" s="8">
-        <v>1</v>
-      </c>
-      <c r="G9" s="8">
-        <v>1</v>
-      </c>
-      <c r="H9" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="17">
+        <v>1</v>
+      </c>
+      <c r="G9" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="28" t="s">
         <v>20</v>
       </c>
@@ -1990,19 +1960,16 @@
         <v>0</v>
       </c>
       <c r="E10" s="8">
-        <v>1</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0</v>
-      </c>
-      <c r="G10" s="8">
-        <v>0</v>
-      </c>
-      <c r="H10" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="17">
+        <v>0</v>
+      </c>
+      <c r="G10" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="28" t="s">
         <v>21</v>
       </c>
@@ -2016,19 +1983,16 @@
         <v>0</v>
       </c>
       <c r="E11" s="8">
-        <v>1</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0</v>
-      </c>
-      <c r="G11" s="8">
-        <v>0</v>
-      </c>
-      <c r="H11" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="F11" s="17">
+        <v>1</v>
+      </c>
+      <c r="G11" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="28" t="s">
         <v>22</v>
       </c>
@@ -2044,17 +2008,14 @@
       <c r="E12" s="8">
         <v>1</v>
       </c>
-      <c r="F12" s="8">
-        <v>0</v>
-      </c>
-      <c r="G12" s="8">
-        <v>1</v>
-      </c>
-      <c r="H12" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="F12" s="17">
+        <v>0</v>
+      </c>
+      <c r="G12" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="28" t="s">
         <v>23</v>
       </c>
@@ -2070,17 +2031,14 @@
       <c r="E13" s="8">
         <v>1</v>
       </c>
-      <c r="F13" s="8">
-        <v>0</v>
-      </c>
-      <c r="G13" s="8">
-        <v>1</v>
-      </c>
-      <c r="H13" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="F13" s="17">
+        <v>1</v>
+      </c>
+      <c r="G13" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="28" t="s">
         <v>24</v>
       </c>
@@ -2094,19 +2052,16 @@
         <v>0</v>
       </c>
       <c r="E14" s="8">
-        <v>1</v>
-      </c>
-      <c r="F14" s="8">
-        <v>1</v>
-      </c>
-      <c r="G14" s="8">
-        <v>0</v>
-      </c>
-      <c r="H14" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0</v>
+      </c>
+      <c r="G14" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="28" t="s">
         <v>25</v>
       </c>
@@ -2120,19 +2075,16 @@
         <v>0</v>
       </c>
       <c r="E15" s="8">
-        <v>1</v>
-      </c>
-      <c r="F15" s="8">
-        <v>1</v>
-      </c>
-      <c r="G15" s="8">
-        <v>0</v>
-      </c>
-      <c r="H15" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="F15" s="17">
+        <v>1</v>
+      </c>
+      <c r="G15" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="28" t="s">
         <v>26</v>
       </c>
@@ -2148,17 +2100,14 @@
       <c r="E16" s="8">
         <v>1</v>
       </c>
-      <c r="F16" s="8">
-        <v>1</v>
-      </c>
-      <c r="G16" s="8">
-        <v>1</v>
-      </c>
-      <c r="H16" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="F16" s="17">
+        <v>0</v>
+      </c>
+      <c r="G16" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="28" t="s">
         <v>27</v>
       </c>
@@ -2174,17 +2123,14 @@
       <c r="E17" s="8">
         <v>1</v>
       </c>
-      <c r="F17" s="8">
-        <v>1</v>
-      </c>
-      <c r="G17" s="8">
-        <v>1</v>
-      </c>
-      <c r="H17" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="F17" s="17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="28" t="s">
         <v>28</v>
       </c>
@@ -2200,17 +2146,14 @@
       <c r="E18" s="8">
         <v>0</v>
       </c>
-      <c r="F18" s="8">
-        <v>0</v>
-      </c>
-      <c r="G18" s="8">
-        <v>0</v>
-      </c>
-      <c r="H18" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="F18" s="17">
+        <v>0</v>
+      </c>
+      <c r="G18" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="28" t="s">
         <v>29</v>
       </c>
@@ -2226,17 +2169,14 @@
       <c r="E19" s="8">
         <v>0</v>
       </c>
-      <c r="F19" s="8">
-        <v>0</v>
-      </c>
-      <c r="G19" s="8">
-        <v>0</v>
-      </c>
-      <c r="H19" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="F19" s="17">
+        <v>1</v>
+      </c>
+      <c r="G19" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="28" t="s">
         <v>30</v>
       </c>
@@ -2250,19 +2190,16 @@
         <v>1</v>
       </c>
       <c r="E20" s="8">
-        <v>0</v>
-      </c>
-      <c r="F20" s="8">
-        <v>0</v>
-      </c>
-      <c r="G20" s="8">
-        <v>1</v>
-      </c>
-      <c r="H20" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="F20" s="17">
+        <v>0</v>
+      </c>
+      <c r="G20" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="28" t="s">
         <v>31</v>
       </c>
@@ -2276,19 +2213,16 @@
         <v>1</v>
       </c>
       <c r="E21" s="8">
-        <v>0</v>
-      </c>
-      <c r="F21" s="8">
-        <v>0</v>
-      </c>
-      <c r="G21" s="8">
-        <v>1</v>
-      </c>
-      <c r="H21" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="F21" s="17">
+        <v>1</v>
+      </c>
+      <c r="G21" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="28" t="s">
         <v>32</v>
       </c>
@@ -2304,17 +2238,14 @@
       <c r="E22" s="8">
         <v>0</v>
       </c>
-      <c r="F22" s="8">
-        <v>1</v>
-      </c>
-      <c r="G22" s="8">
-        <v>0</v>
-      </c>
-      <c r="H22" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="F22" s="17">
+        <v>0</v>
+      </c>
+      <c r="G22" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="28" t="s">
         <v>33</v>
       </c>
@@ -2330,17 +2261,14 @@
       <c r="E23" s="8">
         <v>0</v>
       </c>
-      <c r="F23" s="8">
-        <v>1</v>
-      </c>
-      <c r="G23" s="8">
-        <v>0</v>
-      </c>
-      <c r="H23" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="F23" s="17">
+        <v>1</v>
+      </c>
+      <c r="G23" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="28" t="s">
         <v>34</v>
       </c>
@@ -2354,19 +2282,16 @@
         <v>1</v>
       </c>
       <c r="E24" s="8">
-        <v>0</v>
-      </c>
-      <c r="F24" s="8">
-        <v>1</v>
-      </c>
-      <c r="G24" s="8">
-        <v>1</v>
-      </c>
-      <c r="H24" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="F24" s="17">
+        <v>0</v>
+      </c>
+      <c r="G24" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="28" t="s">
         <v>35</v>
       </c>
@@ -2380,19 +2305,16 @@
         <v>1</v>
       </c>
       <c r="E25" s="8">
-        <v>0</v>
-      </c>
-      <c r="F25" s="8">
-        <v>1</v>
-      </c>
-      <c r="G25" s="8">
-        <v>1</v>
-      </c>
-      <c r="H25" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>1</v>
+      </c>
+      <c r="F25" s="17">
+        <v>1</v>
+      </c>
+      <c r="G25" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="28" t="s">
         <v>36</v>
       </c>
@@ -2406,19 +2328,16 @@
         <v>1</v>
       </c>
       <c r="E26" s="8">
-        <v>1</v>
-      </c>
-      <c r="F26" s="8">
-        <v>0</v>
-      </c>
-      <c r="G26" s="8">
-        <v>0</v>
-      </c>
-      <c r="H26" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="F26" s="17">
+        <v>0</v>
+      </c>
+      <c r="G26" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="28" t="s">
         <v>37</v>
       </c>
@@ -2432,19 +2351,16 @@
         <v>1</v>
       </c>
       <c r="E27" s="8">
-        <v>1</v>
-      </c>
-      <c r="F27" s="8">
-        <v>0</v>
-      </c>
-      <c r="G27" s="8">
-        <v>0</v>
-      </c>
-      <c r="H27" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="F27" s="17">
+        <v>1</v>
+      </c>
+      <c r="G27" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="28" t="s">
         <v>12</v>
       </c>
@@ -2460,17 +2376,14 @@
       <c r="E28" s="8">
         <v>1</v>
       </c>
-      <c r="F28" s="8">
-        <v>0</v>
-      </c>
-      <c r="G28" s="8">
-        <v>1</v>
-      </c>
-      <c r="H28" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="F28" s="17">
+        <v>0</v>
+      </c>
+      <c r="G28" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="28" t="s">
         <v>38</v>
       </c>
@@ -2486,17 +2399,14 @@
       <c r="E29" s="8">
         <v>1</v>
       </c>
-      <c r="F29" s="8">
-        <v>0</v>
-      </c>
-      <c r="G29" s="8">
-        <v>1</v>
-      </c>
-      <c r="H29" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="F29" s="17">
+        <v>1</v>
+      </c>
+      <c r="G29" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="28" t="s">
         <v>39</v>
       </c>
@@ -2510,19 +2420,16 @@
         <v>1</v>
       </c>
       <c r="E30" s="8">
-        <v>1</v>
-      </c>
-      <c r="F30" s="8">
-        <v>1</v>
-      </c>
-      <c r="G30" s="8">
-        <v>0</v>
-      </c>
-      <c r="H30" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="F30" s="17">
+        <v>0</v>
+      </c>
+      <c r="G30" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="28" t="s">
         <v>15</v>
       </c>
@@ -2536,19 +2443,16 @@
         <v>1</v>
       </c>
       <c r="E31" s="8">
-        <v>1</v>
-      </c>
-      <c r="F31" s="8">
-        <v>1</v>
-      </c>
-      <c r="G31" s="8">
-        <v>0</v>
-      </c>
-      <c r="H31" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="F31" s="17">
+        <v>1</v>
+      </c>
+      <c r="G31" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="28" t="s">
         <v>40</v>
       </c>
@@ -2564,17 +2468,14 @@
       <c r="E32" s="8">
         <v>1</v>
       </c>
-      <c r="F32" s="8">
-        <v>1</v>
-      </c>
-      <c r="G32" s="8">
-        <v>1</v>
-      </c>
-      <c r="H32" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="F32" s="17">
+        <v>0</v>
+      </c>
+      <c r="G32" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="33" t="s">
         <v>41</v>
       </c>
@@ -2590,47 +2491,25 @@
       <c r="E33" s="19">
         <v>1</v>
       </c>
-      <c r="F33" s="19">
-        <v>1</v>
-      </c>
-      <c r="G33" s="19">
-        <v>1</v>
-      </c>
-      <c r="H33" s="20">
+      <c r="F33" s="20">
+        <v>1</v>
+      </c>
+      <c r="G33" s="35">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:H500 I2:AP499">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+  <conditionalFormatting sqref="G2:AN499 D2:F500">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:XFD1048576 D34:D1048576">
-      <formula1>0</formula1>
-      <formula2>1</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D33">
-      <formula1>"0,1"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>requirements!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>D1:S1</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>

</xml_diff>